<commit_message>
Ideas of features: Updating vision features to match new vision system
Cf https://hackaday.io/project/26943-evolartist/log/68697-perception-system
</commit_message>
<xml_diff>
--- a/ideas/creatureFeatures.xlsx
+++ b/ideas/creatureFeatures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25440" windowHeight="14620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25440" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,304 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="141">
   <si>
+    <t>visionCapHighLight=8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visionCapHighLight=0; visionCapLowLight=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visionCapHighLight=5; defenseSkill-=1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visionCapHighLight=3; visionCapLowLight=3; defenseSkill+=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visionCapHighLight=1; visionCapLowLight=3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision one spot around in high intensity light. Enable far way vision in low intensity light.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ageDamage = 2 at birth; when age &gt; lifeExpectancy: for each turn: ageDamage += ceil(ageDamage / 2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBDDCD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No aging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Age does not have any impact on health but sickly creature who cannot reproduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low maximum health. Cannot reproduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maxHealth &lt; 25; maxBabies = 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBDDDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creates own light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creates own super powerful light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modify environment -&gt; Turn dark into light one spot around. Looses energy faster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modify environment -&gt; Turn dark into light in the full vision field. Looses energy very fast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glowy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shiny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slower creature but old age has very little impact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loses health very slowly once life expectancy is over. Reduced movement abilities from birth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ageDamage = 2; movementCap -= 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBDDBD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A pair of moustaches to sense the air, cumulative</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A pair of long moustaches to sense the air far away. Cumulative but too many are an hindrance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Some aesthetic characteristic with no impact on fitness, cumulative</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Some aesthetic characteristic with no impact on fitness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sporadic aging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Old has a very random impact on creature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable far away vision in high intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision a few spots around in high intensity light. More damage if attacked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision a few spots around in high and low intensity light. Less damage when attacked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PR1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No impact on fitness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fancy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCBCBB</t>
+  </si>
+  <si>
+    <t>Lifetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The longer the gene, the longer the life</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length of gene determines life expectancy, after which health decreases at each turn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D, DD, DDD, DDDD, DDDDD, DDDDDD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fast aging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loses health very quickly once life expectancy is over</t>
+  </si>
+  <si>
+    <t>Sick when old</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ageDamage = 30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBDDCC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LETHAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Very slow aging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VOID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Void</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lethal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBBB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBDD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBCC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBCD, BBBD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moustaches</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MO1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Long moustaches</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MO2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movesenseCap = 1; movesenseProb += 0.1 per pair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movesenseCap = 3; movesenseProb += 0.1 per pair; visionCap -= 2 if more than 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Regular vision in all lights, protection from attacks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Vision not affected by night one spot away from creature; energyLoss += 3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -78,119 +376,162 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ageDamage = 2 at birth; when age &gt; lifeExpectancy: for each turn: ageDamage += ceil(ageDamage / 2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBDDCD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>No aging</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Age does not have any impact on health but sickly creature who cannot reproduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Low maximum health. Cannot reproduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>maxHealth &lt; 25; maxBabies = 0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBDDDB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Creates own light</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LI1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LI2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Creates own super powerful light</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modify environment -&gt; Turn dark into light one spot around. Looses energy faster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modify environment -&gt; Turn dark into light in the full vision field. Looses energy very fast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Glowy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shiny</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Slower creature but old age has very little impact</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Loses health very slowly once life expectancy is over. Reduced movement abilities from birth</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ageDamage = 2; movementCap -= 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBDDBD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A pair of moustaches to sense the air, cumulative</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A pair of long moustaches to sense the air far away. Cumulative but too many are an hindrance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Some aesthetic characteristic with no impact on fitness, cumulative</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Some aesthetic characteristic with no impact on fitness</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sporadic aging</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Old has a very random impact on creature</t>
+    <t>Good vision but susceptible to attacks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bad day vision but terrific night vision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EX1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Narrative</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Short hairs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Example long</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EX2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Long hairs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Functional description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Better for cold weather, slow dow creature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Simulation modifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Representation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Short hairs on creature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Long hairs on creature + rustling sounds when moving</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Files (art, details…)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Example</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Better for mild to cold weather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sharp eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Best day vision</t>
+  </si>
+  <si>
+    <t>Blind eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eyes that do not work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non-functional eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entirely white eyes?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Globular eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shuttered eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can sense moving things one spot around. Can have multiple of them for improved sensitivity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can sense moving things a few spots around. Can have multiple of them for improved sensitivity. Too many cause diminished vision</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -239,347 +580,6 @@
   </si>
   <si>
     <t>Pretty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PR1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>No impact on fitness</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fancy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FA1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BCBCBB</t>
-  </si>
-  <si>
-    <t>Lifetime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LT1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The longer the gene, the longer the life</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Length of gene determines life expectancy, after which health decreases at each turn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D, DD, DDD, DDDD, DDDDD, DDDDDD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fast aging</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Loses health very quickly once life expectancy is over</t>
-  </si>
-  <si>
-    <t>Sick when old</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ageDamage = 30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBDDCC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LETHAL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Very slow aging</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VOID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Void</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lethal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gene</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBBB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBDD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBBC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBCC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBCD, BBBD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Moustaches</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MO1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Long moustaches</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MO2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Can sense moving things one spot around. Can have multiple of them for improve sensitivity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Can sense moving things a few spots around. Can have multiple of them for improve sensitivity. Too many cause diminished vision</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movesenseCap = 1; movesenseProb += 0.1 per pair</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movesenseCap = 3; movesenseProb += 0.1 per pair; visionCap -= 2 if more than 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Regular vision in all lights, protection from attacks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Can see all objects, far away, in day light</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Can see a few spots around, all objects, in day light. More damage if attacked</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Can see a few spots around, all objects, in all light. Less damage when attacked</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>visionCap=5; defenseSkill-=1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Good vision but susceptible to attacks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bad day vision but terrific night vision</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>visionCap=3; defenseSkill+=1; nightVisionMult = 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Can see one spot around in day light, all objects, can see all object far away in night light</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>visionCap=1; nightVisionMutl=8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EX1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Narrative</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Short hairs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Example long</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EX2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Long hairs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Functional description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Better for cold weather, slow dow creature</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Simulation modifier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gene</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Representation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Short hairs on creature</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Long hairs on creature + rustling sounds when moving</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Files (art, details…)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Example</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Better for mild to cold weather</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sharp eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Best day vision</t>
-  </si>
-  <si>
-    <t>visionCap=8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Blind eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eyes that do not work</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Non-functional eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>visionCap=0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entirely white eyes?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Globular eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shuttered eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Length</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -653,7 +653,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="2">
     <dxf>
       <font>
         <condense val="0"/>
@@ -663,41 +663,6 @@
       <fill>
         <patternFill>
           <bgColor indexed="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1035,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1053,429 +1018,428 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="14" customHeight="1" thickTop="1">
       <c r="A2" s="2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>102</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>140</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="s">
-        <v>56</v>
-      </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="F17" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="F20" t="s">
-        <v>45</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>133</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>134</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>135</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E30" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="F30" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="F31" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1491,7 +1455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:P730"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1508,7 +1472,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1529,42 +1493,42 @@
         <v>6</v>
       </c>
       <c r="N1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="O1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="P1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="B2" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)))</f>
         <v>BB</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="F2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)) )</f>
         <v>BBB</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)), IF(MOD(QUOTIENT(ROW() - 2,27),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)) )</f>
         <v>BBBB</v>
       </c>
       <c r="I2" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,27),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,81),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,81), 3) = 1, $B$3, $B$4)) )</f>
@@ -1589,20 +1553,20 @@
     </row>
     <row r="3" spans="1:16">
       <c r="B3" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D9" si="0">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)))</f>
         <v>CB</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F36" si="1">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)) )</f>
+        <f t="shared" ref="F3:F27" si="1">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)) )</f>
         <v>CBB</v>
       </c>
       <c r="H3" t="str">
@@ -1620,17 +1584,17 @@
     </row>
     <row r="4" spans="1:16">
       <c r="B4" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>DB</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -1655,7 +1619,7 @@
         <v>BC</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -1666,14 +1630,14 @@
         <v>BCBB</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="3"/>
         <v>BCBBB</v>
       </c>
       <c r="K5" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="4"/>
@@ -1686,7 +1650,7 @@
         <v>CC</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
@@ -1711,7 +1675,7 @@
         <v>DC</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
@@ -1736,7 +1700,7 @@
         <v>BD</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
@@ -1761,7 +1725,7 @@
         <v>CD</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -1786,7 +1750,7 @@
         <v>DD</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -1811,7 +1775,7 @@
         <v>BBC</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="2"/>
@@ -1872,14 +1836,14 @@
         <v>BCCB</v>
       </c>
       <c r="I14" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="3"/>
         <v>BCCBB</v>
       </c>
       <c r="K14" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="4"/>
@@ -1982,7 +1946,7 @@
         <v>BBD</v>
       </c>
       <c r="G20" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="2"/>
@@ -2043,14 +2007,14 @@
         <v>BCDB</v>
       </c>
       <c r="I23" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="3"/>
         <v>BCDBB</v>
       </c>
       <c r="K23" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="4"/>
@@ -2135,7 +2099,7 @@
         <v>DDD</v>
       </c>
       <c r="G28" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="2"/>
@@ -2156,7 +2120,7 @@
         <v>BBBC</v>
       </c>
       <c r="I29" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="3"/>
@@ -2209,7 +2173,7 @@
         <v>BCBCBB</v>
       </c>
       <c r="M32" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="8:12">
@@ -2288,7 +2252,7 @@
         <v>BBCC</v>
       </c>
       <c r="I38" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="3"/>
@@ -2463,7 +2427,7 @@
         <v>BCDCB</v>
       </c>
       <c r="K50" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="L50" t="str">
         <f t="shared" si="4"/>
@@ -2546,7 +2510,7 @@
         <v>BBBD</v>
       </c>
       <c r="I56" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="J56" t="str">
         <f t="shared" si="3"/>
@@ -2675,7 +2639,7 @@
         <v>BBCD</v>
       </c>
       <c r="I65" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="J65" t="str">
         <f t="shared" si="3"/>
@@ -2804,7 +2768,7 @@
         <v>BBDD</v>
       </c>
       <c r="I74" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J74" t="str">
         <f t="shared" si="6"/>
@@ -2919,7 +2883,7 @@
         <v>DDDD</v>
       </c>
       <c r="I82" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="J82" t="str">
         <f t="shared" si="6"/>
@@ -4470,7 +4434,7 @@
         <v>BBDDDB</v>
       </c>
       <c r="M236" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="237" spans="10:13">
@@ -4549,7 +4513,7 @@
         <v>DDDDD</v>
       </c>
       <c r="K244" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="L244" t="str">
         <f t="shared" si="11"/>
@@ -4558,7 +4522,7 @@
     </row>
     <row r="245" spans="10:12">
       <c r="L245" t="str">
-        <f t="shared" ref="L195:L258" si="12">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,81),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,81), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,243),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,243), 3) = 1, $B$3, $B$4)))</f>
+        <f t="shared" ref="L245:L258" si="12">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,81),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,81), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,243),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,243), 3) = 1, $B$3, $B$4)))</f>
         <v>BBBBBC</v>
       </c>
     </row>
@@ -4994,7 +4958,7 @@
         <v>BBDDBC</v>
       </c>
       <c r="M317" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="318" spans="12:13">
@@ -5483,7 +5447,7 @@
         <v>BBDDCC</v>
       </c>
       <c r="M398" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="399" spans="12:13">
@@ -6458,7 +6422,7 @@
         <v>BBDDBD</v>
       </c>
       <c r="M560" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="561" spans="12:12">
@@ -6947,7 +6911,7 @@
         <v>BBDDCD</v>
       </c>
       <c r="M641" t="s">
-        <v>47</v>
+        <v>133</v>
       </c>
     </row>
     <row r="642" spans="12:13">
@@ -7342,7 +7306,7 @@
     </row>
     <row r="707" spans="12:12">
       <c r="L707" t="str">
-        <f t="shared" ref="L707:L735" si="20">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,81),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,81), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,243),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,243), 3) = 1, $B$3, $B$4)))</f>
+        <f t="shared" ref="L707:L730" si="20">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,81),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,81), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,243),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,243), 3) = 1, $B$3, $B$4)))</f>
         <v>BCBDDD</v>
       </c>
     </row>
@@ -7484,11 +7448,10 @@
         <v>DDDDDD</v>
       </c>
       <c r="M730" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="M642:M1048576 N1:XFD1048576 M1:M316 M318:M640 A1:L1048576">
     <cfRule type="cellIs" dxfId="1" priority="0" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
Ideas of features: Adding features for colored vision
</commit_message>
<xml_diff>
--- a/ideas/creatureFeatures.xlsx
+++ b/ideas/creatureFeatures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25440" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25440" windowHeight="14620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,566 +20,793 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="199">
+  <si>
+    <t>Example long</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EX2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Long hairs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Functional description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Better for cold weather, slow dow creature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Simulation modifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Representation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Short hairs on creature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Long hairs on creature + rustling sounds when moving</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Files (art, details…)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Example</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Better for mild to cold weather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sharp eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Best day vision</t>
+  </si>
+  <si>
+    <t>Blind eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eyes that do not work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non-functional eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entirely white eyes?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Globular eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shuttered eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can sense moving things one spot around. Can have multiple of them for improved sensitivity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can sense moving things a few spots around. Can have multiple of them for improved sensitivity. Too many cause diminished vision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ageDamage in [5, 50]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fix the age damage randomly at birth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBDDBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Progressive aging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creature becomes sicker as it ages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loses more and more health each turn once life expectancy is over</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VOID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BB, BC, BD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pretty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCCDBB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCDDBB, BCBDBB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DCCDBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DBBCDB, DCCCDB, DDDCDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DCBDBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision a few spots around in high and low intensity light. Less damage when attacked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PR1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No impact on fitness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fancy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCBCBB</t>
+  </si>
+  <si>
+    <t>Lifetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The longer the gene, the longer the life</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length of gene determines life expectancy, after which health decreases at each turn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D, DD, DDD, DDDD, DDDDD, DDDDDD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fast aging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loses health very quickly once life expectancy is over</t>
+  </si>
+  <si>
+    <t>Sick when old</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ageDamage = 30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBDDCC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LETHAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Very slow aging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VOID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Void</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lethal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBBB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBDD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBCC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBCD, BBBD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moustaches</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MO1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Long moustaches</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MO2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movesenseCap = 1; movesenseProb += 0.1 per pair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movesenseCap = 3; movesenseProb += 0.1 per pair; visionCap -= 2 if more than 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Regular vision in all lights, protection from attacks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vision not affected by night one spot away from creature; energyLoss += 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vision not affected by night; energyLoss += 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCDBB, BCCBB, BCBBB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LT2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCDCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blushy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creates very low light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Looses very little energy to sustain the light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>energyLoss += 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCDB, BCCB, BCBB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lifeExpectancy = 15*length of gene; when age &gt; lifeExpectancy: for each turn: health -= ageDamage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Good vision but susceptible to attacks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EY5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bad day vision but terrific night vision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EX1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Narrative</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Short hairs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visionCapHighLight=5; defenseSkill-=1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visionCapHighLight=3; visionCapLowLight=3; defenseSkill+=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visionCapHighLight=1; visionCapLowLight=3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision one spot around in high intensity light. Enable far way vision in low intensity light.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modify environment -&gt; Turn low into high intensity light one spot around. Looses energy faster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modify environment -&gt; Turn  low into high intensity light in the full vision field. Looses energy very fast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rainbow eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can see all colors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ageDamage = 2 at birth; when age &gt; lifeExpectancy: for each turn: ageDamage += ceil(ageDamage / 2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBDDCD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No aging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Age does not have any impact on health but sickly creature who cannot reproduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low maximum health. Cannot reproduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maxHealth &lt; 25; maxBabies = 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBDDDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creates own light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creates own super powerful light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glowy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shiny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slower creature but old age has very little impact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loses health very slowly once life expectancy is over. Reduced movement abilities from birth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ageDamage = 2; movementCap -= 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBDDBD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A pair of moustaches to sense the air, cumulative</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A pair of long moustaches to sense the air far away. Cumulative but too many are an hindrance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Some aesthetic characteristic with no impact on fitness, cumulative</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Some aesthetic characteristic with no impact on fitness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sporadic aging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Old has a very random impact on creature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable far away vision in high intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision a few spots around in high intensity light. More damage if attacked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision = [(3, 5), (-1, -1), (-1, -1)]; Red capped (lower) at 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision = [(0, 3), (0, 3), (0, 3)]; all colors capped (upper) at 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision for green and low levels and red and blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision = [(0, 1), (0, 2), (0, 5)]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCCDBB, CCCDBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DCCDBB</t>
+  </si>
+  <si>
+    <t>VI7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDCDBB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision for mid levels of blue and green</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision = [(-1, -1), (1, 3), (2, 4)]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aubergine eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI3</t>
+  </si>
+  <si>
+    <t>VI4</t>
+  </si>
+  <si>
+    <t>VI5</t>
+  </si>
+  <si>
+    <t>VI6</t>
+  </si>
+  <si>
+    <t>Can see blue and green</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can see red and some blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision for high levels of red and low levels of blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision = [(3, 5), (-1, -1), (0, 2)]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can see very high and very low levels of red, blue and green</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision for very high and very low levels of red, blue and green</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision = [(0, 1)U(4,5), (0, 1)U(4,5), (0, 1)U(4,5)]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Limit eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pasture eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can see green and low levels of red and blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision = [(-1, -1), (-1, -1), (0, 5)]; block red and green values</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision for all colors. Looses energy faster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision = [(0, 5), (0, 5), (0, 5)]; energyLoss += 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ocean eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can only see blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision for blue. Stops all colors.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baby eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can only see lower levels of colors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision for all colors but stops high levels of colors.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red blood eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Night eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can only see high levels of red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable vision for high level of red, stops low levels of red.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turquoise eyes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>visionCapHighLight=8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>visionCapHighLight=0; visionCapLowLight=0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>visionCapHighLight=5; defenseSkill-=1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>visionCapHighLight=3; visionCapLowLight=3; defenseSkill+=1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>visionCapHighLight=1; visionCapLowLight=3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable vision one spot around in high intensity light. Enable far way vision in low intensity light.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ageDamage = 2 at birth; when age &gt; lifeExpectancy: for each turn: ageDamage += ceil(ageDamage / 2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBDDCD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>No aging</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Age does not have any impact on health but sickly creature who cannot reproduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Low maximum health. Cannot reproduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>maxHealth &lt; 25; maxBabies = 0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBDDDB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Creates own light</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LI1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LI2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Creates own super powerful light</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modify environment -&gt; Turn dark into light one spot around. Looses energy faster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modify environment -&gt; Turn dark into light in the full vision field. Looses energy very fast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Glowy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shiny</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Slower creature but old age has very little impact</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Loses health very slowly once life expectancy is over. Reduced movement abilities from birth</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ageDamage = 2; movementCap -= 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBDDBD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A pair of moustaches to sense the air, cumulative</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A pair of long moustaches to sense the air far away. Cumulative but too many are an hindrance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Some aesthetic characteristic with no impact on fitness, cumulative</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Some aesthetic characteristic with no impact on fitness</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sporadic aging</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Old has a very random impact on creature</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable far away vision in high intensity light</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable vision a few spots around in high intensity light. More damage if attacked</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable vision a few spots around in high and low intensity light. Less damage when attacked</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PR1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>No impact on fitness</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fancy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FA1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BCBCBB</t>
-  </si>
-  <si>
-    <t>Lifetime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LT1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The longer the gene, the longer the life</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Length of gene determines life expectancy, after which health decreases at each turn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D, DD, DDD, DDDD, DDDDD, DDDDDD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fast aging</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Loses health very quickly once life expectancy is over</t>
-  </si>
-  <si>
-    <t>Sick when old</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ageDamage = 30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBDDCC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LETHAL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Very slow aging</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VOID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Void</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lethal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gene</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBBB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBDD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBBC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBCC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBCD, BBBD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Moustaches</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MO1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Long moustaches</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MO2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movesenseCap = 1; movesenseProb += 0.1 per pair</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movesenseCap = 3; movesenseProb += 0.1 per pair; visionCap -= 2 if more than 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Regular vision in all lights, protection from attacks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vision not affected by night one spot away from creature; energyLoss += 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vision not affected by night; energyLoss += 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LI1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BCDBB, BCCBB, BCBBB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LT2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BCDCB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Blushy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LI3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Creates very low light</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Looses very little energy to sustain the light</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>energyLoss += 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BCDB, BCCB, BCBB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LI3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lifeExpectancy = 15*length of gene; when age &gt; lifeExpectancy: for each turn: health -= ageDamage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Good vision but susceptible to attacks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bad day vision but terrific night vision</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EX1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Narrative</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Short hairs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Example long</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EX2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Long hairs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Functional description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Better for cold weather, slow dow creature</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Simulation modifier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gene</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Representation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Short hairs on creature</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Long hairs on creature + rustling sounds when moving</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Files (art, details…)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Example</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Better for mild to cold weather</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sharp eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Best day vision</t>
-  </si>
-  <si>
-    <t>Blind eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eyes that do not work</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Non-functional eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entirely white eyes?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Globular eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shuttered eyes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EY4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Length</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Can sense moving things one spot around. Can have multiple of them for improved sensitivity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Can sense moving things a few spots around. Can have multiple of them for improved sensitivity. Too many cause diminished vision</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ageDamage in [5, 50]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fix the age damage randomly at birth</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBDDBC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Progressive aging</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AG4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Creature becomes sicker as it ages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Loses more and more health each turn once life expectancy is over</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VOID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BB, BC, BD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pretty</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -998,448 +1225,609 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView view="pageLayout" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="97" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="78" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>105</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>108</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="14" customHeight="1" thickTop="1">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>106</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>149</v>
       </c>
       <c r="E5" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>198</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="G6" t="s">
-        <v>118</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>117</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>166</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>188</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>183</v>
       </c>
       <c r="F11" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>189</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>167</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>190</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>191</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>152</v>
       </c>
       <c r="F12" t="s">
-        <v>137</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" t="s">
+        <v>195</v>
+      </c>
+      <c r="E13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>196</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>169</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>171</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>162</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
       <c r="F14" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>164</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>172</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>173</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>174</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" t="s">
+        <v>176</v>
+      </c>
+      <c r="D16" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>180</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>182</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" t="s">
         <v>52</v>
-      </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>142</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="D20" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>132</v>
-      </c>
-      <c r="B21" t="s">
-        <v>133</v>
-      </c>
-      <c r="C21" t="s">
-        <v>134</v>
-      </c>
-      <c r="D21" t="s">
-        <v>135</v>
-      </c>
-      <c r="E21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>144</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
       <c r="F30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" t="s">
-        <v>85</v>
-      </c>
-      <c r="F32" t="s">
-        <v>86</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" t="s">
+        <v>118</v>
+      </c>
+      <c r="E38" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" t="s">
+        <v>93</v>
+      </c>
+      <c r="F39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1455,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:P730"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="M306" sqref="M306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1472,7 +1860,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1493,42 +1881,42 @@
         <v>6</v>
       </c>
       <c r="N1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="O1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="P1" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="B2" t="s">
-        <v>123</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)))</f>
         <v>BB</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)) )</f>
         <v>BBB</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)), IF(MOD(QUOTIENT(ROW() - 2,27),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)) )</f>
         <v>BBBB</v>
       </c>
       <c r="I2" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="J2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,27),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,81),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,81), 3) = 1, $B$3, $B$4)) )</f>
@@ -1548,22 +1936,22 @@
       </c>
       <c r="P2">
         <f>COUNTIF($C$2:$C$4,"*")+O2+COUNTIF($E$2:$E$10,"*")+COUNTIF($G$2:$G$28,"*")+COUNTIF($I$2:$I$82,"*")+COUNTIF($K$2:$K$244,"*")+COUNTIF($M$2:$M$730,"*") - N2 - O2</f>
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="B3" t="s">
-        <v>124</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D9" si="0">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)))</f>
         <v>CB</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
+        <v>40</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F27" si="1">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)) )</f>
@@ -1584,17 +1972,17 @@
     </row>
     <row r="4" spans="1:16">
       <c r="B4" t="s">
-        <v>125</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>DB</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -1619,7 +2007,7 @@
         <v>BC</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -1630,14 +2018,14 @@
         <v>BCBB</v>
       </c>
       <c r="I5" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="3"/>
         <v>BCBBB</v>
       </c>
       <c r="K5" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="4"/>
@@ -1650,7 +2038,7 @@
         <v>CC</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
@@ -1675,7 +2063,7 @@
         <v>DC</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
@@ -1700,7 +2088,7 @@
         <v>BD</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
@@ -1725,7 +2113,7 @@
         <v>CD</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -1750,7 +2138,7 @@
         <v>DD</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -1775,7 +2163,7 @@
         <v>BBC</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="2"/>
@@ -1836,14 +2224,14 @@
         <v>BCCB</v>
       </c>
       <c r="I14" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="3"/>
         <v>BCCBB</v>
       </c>
       <c r="K14" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="4"/>
@@ -1946,7 +2334,7 @@
         <v>BBD</v>
       </c>
       <c r="G20" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="2"/>
@@ -2007,14 +2395,14 @@
         <v>BCDB</v>
       </c>
       <c r="I23" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="3"/>
         <v>BCDBB</v>
       </c>
       <c r="K23" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="4"/>
@@ -2099,7 +2487,7 @@
         <v>DDD</v>
       </c>
       <c r="G28" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="2"/>
@@ -2120,7 +2508,7 @@
         <v>BBBC</v>
       </c>
       <c r="I29" t="s">
-        <v>122</v>
+        <v>24</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="3"/>
@@ -2173,7 +2561,7 @@
         <v>BCBCBB</v>
       </c>
       <c r="M32" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="8:12">
@@ -2252,7 +2640,7 @@
         <v>BBCC</v>
       </c>
       <c r="I38" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="3"/>
@@ -2403,7 +2791,7 @@
         <v>CBDCBB</v>
       </c>
     </row>
-    <row r="49" spans="8:12">
+    <row r="49" spans="8:13">
       <c r="H49" t="str">
         <f t="shared" si="2"/>
         <v>DBDC</v>
@@ -2417,7 +2805,7 @@
         <v>DBDCBB</v>
       </c>
     </row>
-    <row r="50" spans="8:12">
+    <row r="50" spans="8:13">
       <c r="H50" t="str">
         <f t="shared" si="2"/>
         <v>BCDC</v>
@@ -2427,14 +2815,14 @@
         <v>BCDCB</v>
       </c>
       <c r="K50" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="L50" t="str">
         <f t="shared" si="4"/>
         <v>BCDCBB</v>
       </c>
     </row>
-    <row r="51" spans="8:12">
+    <row r="51" spans="8:13">
       <c r="H51" t="str">
         <f t="shared" si="2"/>
         <v>CCDC</v>
@@ -2448,7 +2836,7 @@
         <v>CCDCBB</v>
       </c>
     </row>
-    <row r="52" spans="8:12">
+    <row r="52" spans="8:13">
       <c r="H52" t="str">
         <f t="shared" si="2"/>
         <v>DCDC</v>
@@ -2462,7 +2850,7 @@
         <v>DCDCBB</v>
       </c>
     </row>
-    <row r="53" spans="8:12">
+    <row r="53" spans="8:13">
       <c r="H53" t="str">
         <f t="shared" si="2"/>
         <v>BDDC</v>
@@ -2476,7 +2864,7 @@
         <v>BDDCBB</v>
       </c>
     </row>
-    <row r="54" spans="8:12">
+    <row r="54" spans="8:13">
       <c r="H54" t="str">
         <f t="shared" si="2"/>
         <v>CDDC</v>
@@ -2490,7 +2878,7 @@
         <v>CDDCBB</v>
       </c>
     </row>
-    <row r="55" spans="8:12">
+    <row r="55" spans="8:13">
       <c r="H55" t="str">
         <f t="shared" si="2"/>
         <v>DDDC</v>
@@ -2504,13 +2892,13 @@
         <v>DDDCBB</v>
       </c>
     </row>
-    <row r="56" spans="8:12">
+    <row r="56" spans="8:13">
       <c r="H56" t="str">
         <f t="shared" si="2"/>
         <v>BBBD</v>
       </c>
       <c r="I56" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="J56" t="str">
         <f t="shared" si="3"/>
@@ -2521,7 +2909,7 @@
         <v>BBBDBB</v>
       </c>
     </row>
-    <row r="57" spans="8:12">
+    <row r="57" spans="8:13">
       <c r="H57" t="str">
         <f t="shared" si="2"/>
         <v>CBBD</v>
@@ -2535,7 +2923,7 @@
         <v>CBBDBB</v>
       </c>
     </row>
-    <row r="58" spans="8:12">
+    <row r="58" spans="8:13">
       <c r="H58" t="str">
         <f t="shared" si="2"/>
         <v>DBBD</v>
@@ -2549,7 +2937,7 @@
         <v>DBBDBB</v>
       </c>
     </row>
-    <row r="59" spans="8:12">
+    <row r="59" spans="8:13">
       <c r="H59" t="str">
         <f t="shared" si="2"/>
         <v>BCBD</v>
@@ -2562,8 +2950,11 @@
         <f t="shared" si="4"/>
         <v>BCBDBB</v>
       </c>
-    </row>
-    <row r="60" spans="8:12">
+      <c r="M59" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="8:13">
       <c r="H60" t="str">
         <f t="shared" si="2"/>
         <v>CCBD</v>
@@ -2577,7 +2968,7 @@
         <v>CCBDBB</v>
       </c>
     </row>
-    <row r="61" spans="8:12">
+    <row r="61" spans="8:13">
       <c r="H61" t="str">
         <f t="shared" si="2"/>
         <v>DCBD</v>
@@ -2591,7 +2982,7 @@
         <v>DCBDBB</v>
       </c>
     </row>
-    <row r="62" spans="8:12">
+    <row r="62" spans="8:13">
       <c r="H62" t="str">
         <f t="shared" si="2"/>
         <v>BDBD</v>
@@ -2605,7 +2996,7 @@
         <v>BDBDBB</v>
       </c>
     </row>
-    <row r="63" spans="8:12">
+    <row r="63" spans="8:13">
       <c r="H63" t="str">
         <f t="shared" si="2"/>
         <v>CDBD</v>
@@ -2619,7 +3010,7 @@
         <v>CDBDBB</v>
       </c>
     </row>
-    <row r="64" spans="8:12">
+    <row r="64" spans="8:13">
       <c r="H64" t="str">
         <f t="shared" si="2"/>
         <v>DDBD</v>
@@ -2633,13 +3024,13 @@
         <v>DDBDBB</v>
       </c>
     </row>
-    <row r="65" spans="8:12">
+    <row r="65" spans="8:13">
       <c r="H65" t="str">
         <f t="shared" si="2"/>
         <v>BBCD</v>
       </c>
       <c r="I65" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="J65" t="str">
         <f t="shared" si="3"/>
@@ -2650,7 +3041,7 @@
         <v>BBCDBB</v>
       </c>
     </row>
-    <row r="66" spans="8:12">
+    <row r="66" spans="8:13">
       <c r="H66" t="str">
         <f t="shared" si="2"/>
         <v>CBCD</v>
@@ -2664,7 +3055,7 @@
         <v>CBCDBB</v>
       </c>
     </row>
-    <row r="67" spans="8:12">
+    <row r="67" spans="8:13">
       <c r="H67" t="str">
         <f t="shared" ref="H67:H82" si="5">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)), IF(MOD(QUOTIENT(ROW() - 2,27),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)) )</f>
         <v>DBCD</v>
@@ -2678,7 +3069,7 @@
         <v>DBCDBB</v>
       </c>
     </row>
-    <row r="68" spans="8:12">
+    <row r="68" spans="8:13">
       <c r="H68" t="str">
         <f t="shared" si="5"/>
         <v>BCCD</v>
@@ -2691,8 +3082,11 @@
         <f t="shared" si="7"/>
         <v>BCCDBB</v>
       </c>
-    </row>
-    <row r="69" spans="8:12">
+      <c r="M68" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="8:13">
       <c r="H69" t="str">
         <f t="shared" si="5"/>
         <v>CCCD</v>
@@ -2705,8 +3099,11 @@
         <f t="shared" si="7"/>
         <v>CCCDBB</v>
       </c>
-    </row>
-    <row r="70" spans="8:12">
+      <c r="M69" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="70" spans="8:13">
       <c r="H70" t="str">
         <f t="shared" si="5"/>
         <v>DCCD</v>
@@ -2719,8 +3116,11 @@
         <f t="shared" si="7"/>
         <v>DCCDBB</v>
       </c>
-    </row>
-    <row r="71" spans="8:12">
+      <c r="M70" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="71" spans="8:13">
       <c r="H71" t="str">
         <f t="shared" si="5"/>
         <v>BDCD</v>
@@ -2734,7 +3134,7 @@
         <v>BDCDBB</v>
       </c>
     </row>
-    <row r="72" spans="8:12">
+    <row r="72" spans="8:13">
       <c r="H72" t="str">
         <f t="shared" si="5"/>
         <v>CDCD</v>
@@ -2747,8 +3147,11 @@
         <f t="shared" si="7"/>
         <v>CDCDBB</v>
       </c>
-    </row>
-    <row r="73" spans="8:12">
+      <c r="M72" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="73" spans="8:13">
       <c r="H73" t="str">
         <f t="shared" si="5"/>
         <v>DDCD</v>
@@ -2762,13 +3165,13 @@
         <v>DDCDBB</v>
       </c>
     </row>
-    <row r="74" spans="8:12">
+    <row r="74" spans="8:13">
       <c r="H74" t="str">
         <f t="shared" si="5"/>
         <v>BBDD</v>
       </c>
       <c r="I74" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="J74" t="str">
         <f t="shared" si="6"/>
@@ -2779,7 +3182,7 @@
         <v>BBDDBB</v>
       </c>
     </row>
-    <row r="75" spans="8:12">
+    <row r="75" spans="8:13">
       <c r="H75" t="str">
         <f t="shared" si="5"/>
         <v>CBDD</v>
@@ -2793,7 +3196,7 @@
         <v>CBDDBB</v>
       </c>
     </row>
-    <row r="76" spans="8:12">
+    <row r="76" spans="8:13">
       <c r="H76" t="str">
         <f t="shared" si="5"/>
         <v>DBDD</v>
@@ -2807,7 +3210,7 @@
         <v>DBDDBB</v>
       </c>
     </row>
-    <row r="77" spans="8:12">
+    <row r="77" spans="8:13">
       <c r="H77" t="str">
         <f t="shared" si="5"/>
         <v>BCDD</v>
@@ -2820,8 +3223,11 @@
         <f t="shared" si="7"/>
         <v>BCDDBB</v>
       </c>
-    </row>
-    <row r="78" spans="8:12">
+      <c r="M77" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78" spans="8:13">
       <c r="H78" t="str">
         <f t="shared" si="5"/>
         <v>CCDD</v>
@@ -2835,7 +3241,7 @@
         <v>CCDDBB</v>
       </c>
     </row>
-    <row r="79" spans="8:12">
+    <row r="79" spans="8:13">
       <c r="H79" t="str">
         <f t="shared" si="5"/>
         <v>DCDD</v>
@@ -2849,7 +3255,7 @@
         <v>DCDDBB</v>
       </c>
     </row>
-    <row r="80" spans="8:12">
+    <row r="80" spans="8:13">
       <c r="H80" t="str">
         <f t="shared" si="5"/>
         <v>BDDD</v>
@@ -2883,7 +3289,7 @@
         <v>DDDD</v>
       </c>
       <c r="I82" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="J82" t="str">
         <f t="shared" si="6"/>
@@ -3994,7 +4400,7 @@
         <v>CBBCDB</v>
       </c>
     </row>
-    <row r="193" spans="10:12">
+    <row r="193" spans="10:13">
       <c r="J193" t="str">
         <f t="shared" si="8"/>
         <v>DBBCD</v>
@@ -4003,8 +4409,11 @@
         <f t="shared" si="9"/>
         <v>DBBCDB</v>
       </c>
-    </row>
-    <row r="194" spans="10:12">
+      <c r="M193" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="194" spans="10:13">
       <c r="J194" t="str">
         <f t="shared" si="8"/>
         <v>BCBCD</v>
@@ -4014,7 +4423,7 @@
         <v>BCBCDB</v>
       </c>
     </row>
-    <row r="195" spans="10:12">
+    <row r="195" spans="10:13">
       <c r="J195" t="str">
         <f t="shared" ref="J195:J244" si="10">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,27),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,81),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,81), 3) = 1, $B$3, $B$4)) )</f>
         <v>CCBCD</v>
@@ -4024,7 +4433,7 @@
         <v>CCBCDB</v>
       </c>
     </row>
-    <row r="196" spans="10:12">
+    <row r="196" spans="10:13">
       <c r="J196" t="str">
         <f t="shared" si="10"/>
         <v>DCBCD</v>
@@ -4034,7 +4443,7 @@
         <v>DCBCDB</v>
       </c>
     </row>
-    <row r="197" spans="10:12">
+    <row r="197" spans="10:13">
       <c r="J197" t="str">
         <f t="shared" si="10"/>
         <v>BDBCD</v>
@@ -4044,7 +4453,7 @@
         <v>BDBCDB</v>
       </c>
     </row>
-    <row r="198" spans="10:12">
+    <row r="198" spans="10:13">
       <c r="J198" t="str">
         <f t="shared" si="10"/>
         <v>CDBCD</v>
@@ -4054,7 +4463,7 @@
         <v>CDBCDB</v>
       </c>
     </row>
-    <row r="199" spans="10:12">
+    <row r="199" spans="10:13">
       <c r="J199" t="str">
         <f t="shared" si="10"/>
         <v>DDBCD</v>
@@ -4064,7 +4473,7 @@
         <v>DDBCDB</v>
       </c>
     </row>
-    <row r="200" spans="10:12">
+    <row r="200" spans="10:13">
       <c r="J200" t="str">
         <f t="shared" si="10"/>
         <v>BBCCD</v>
@@ -4074,7 +4483,7 @@
         <v>BBCCDB</v>
       </c>
     </row>
-    <row r="201" spans="10:12">
+    <row r="201" spans="10:13">
       <c r="J201" t="str">
         <f t="shared" si="10"/>
         <v>CBCCD</v>
@@ -4084,7 +4493,7 @@
         <v>CBCCDB</v>
       </c>
     </row>
-    <row r="202" spans="10:12">
+    <row r="202" spans="10:13">
       <c r="J202" t="str">
         <f t="shared" si="10"/>
         <v>DBCCD</v>
@@ -4094,7 +4503,7 @@
         <v>DBCCDB</v>
       </c>
     </row>
-    <row r="203" spans="10:12">
+    <row r="203" spans="10:13">
       <c r="J203" t="str">
         <f t="shared" si="10"/>
         <v>BCCCD</v>
@@ -4104,7 +4513,7 @@
         <v>BCCCDB</v>
       </c>
     </row>
-    <row r="204" spans="10:12">
+    <row r="204" spans="10:13">
       <c r="J204" t="str">
         <f t="shared" si="10"/>
         <v>CCCCD</v>
@@ -4114,7 +4523,7 @@
         <v>CCCCDB</v>
       </c>
     </row>
-    <row r="205" spans="10:12">
+    <row r="205" spans="10:13">
       <c r="J205" t="str">
         <f t="shared" si="10"/>
         <v>DCCCD</v>
@@ -4123,8 +4532,11 @@
         <f t="shared" si="11"/>
         <v>DCCCDB</v>
       </c>
-    </row>
-    <row r="206" spans="10:12">
+      <c r="M205" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="206" spans="10:13">
       <c r="J206" t="str">
         <f t="shared" si="10"/>
         <v>BDCCD</v>
@@ -4134,7 +4546,7 @@
         <v>BDCCDB</v>
       </c>
     </row>
-    <row r="207" spans="10:12">
+    <row r="207" spans="10:13">
       <c r="J207" t="str">
         <f t="shared" si="10"/>
         <v>CDCCD</v>
@@ -4144,7 +4556,7 @@
         <v>CDCCDB</v>
       </c>
     </row>
-    <row r="208" spans="10:12">
+    <row r="208" spans="10:13">
       <c r="J208" t="str">
         <f t="shared" si="10"/>
         <v>DDCCD</v>
@@ -4154,7 +4566,7 @@
         <v>DDCCDB</v>
       </c>
     </row>
-    <row r="209" spans="10:12">
+    <row r="209" spans="10:13">
       <c r="J209" t="str">
         <f t="shared" si="10"/>
         <v>BBDCD</v>
@@ -4164,7 +4576,7 @@
         <v>BBDCDB</v>
       </c>
     </row>
-    <row r="210" spans="10:12">
+    <row r="210" spans="10:13">
       <c r="J210" t="str">
         <f t="shared" si="10"/>
         <v>CBDCD</v>
@@ -4174,7 +4586,7 @@
         <v>CBDCDB</v>
       </c>
     </row>
-    <row r="211" spans="10:12">
+    <row r="211" spans="10:13">
       <c r="J211" t="str">
         <f t="shared" si="10"/>
         <v>DBDCD</v>
@@ -4184,7 +4596,7 @@
         <v>DBDCDB</v>
       </c>
     </row>
-    <row r="212" spans="10:12">
+    <row r="212" spans="10:13">
       <c r="J212" t="str">
         <f t="shared" si="10"/>
         <v>BCDCD</v>
@@ -4194,7 +4606,7 @@
         <v>BCDCDB</v>
       </c>
     </row>
-    <row r="213" spans="10:12">
+    <row r="213" spans="10:13">
       <c r="J213" t="str">
         <f t="shared" si="10"/>
         <v>CCDCD</v>
@@ -4204,7 +4616,7 @@
         <v>CCDCDB</v>
       </c>
     </row>
-    <row r="214" spans="10:12">
+    <row r="214" spans="10:13">
       <c r="J214" t="str">
         <f t="shared" si="10"/>
         <v>DCDCD</v>
@@ -4214,7 +4626,7 @@
         <v>DCDCDB</v>
       </c>
     </row>
-    <row r="215" spans="10:12">
+    <row r="215" spans="10:13">
       <c r="J215" t="str">
         <f t="shared" si="10"/>
         <v>BDDCD</v>
@@ -4224,7 +4636,7 @@
         <v>BDDCDB</v>
       </c>
     </row>
-    <row r="216" spans="10:12">
+    <row r="216" spans="10:13">
       <c r="J216" t="str">
         <f t="shared" si="10"/>
         <v>CDDCD</v>
@@ -4234,7 +4646,7 @@
         <v>CDDCDB</v>
       </c>
     </row>
-    <row r="217" spans="10:12">
+    <row r="217" spans="10:13">
       <c r="J217" t="str">
         <f t="shared" si="10"/>
         <v>DDDCD</v>
@@ -4243,8 +4655,11 @@
         <f t="shared" si="11"/>
         <v>DDDCDB</v>
       </c>
-    </row>
-    <row r="218" spans="10:12">
+      <c r="M217" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="218" spans="10:13">
       <c r="J218" t="str">
         <f t="shared" si="10"/>
         <v>BBBDD</v>
@@ -4254,7 +4669,7 @@
         <v>BBBDDB</v>
       </c>
     </row>
-    <row r="219" spans="10:12">
+    <row r="219" spans="10:13">
       <c r="J219" t="str">
         <f t="shared" si="10"/>
         <v>CBBDD</v>
@@ -4264,7 +4679,7 @@
         <v>CBBDDB</v>
       </c>
     </row>
-    <row r="220" spans="10:12">
+    <row r="220" spans="10:13">
       <c r="J220" t="str">
         <f t="shared" si="10"/>
         <v>DBBDD</v>
@@ -4274,7 +4689,7 @@
         <v>DBBDDB</v>
       </c>
     </row>
-    <row r="221" spans="10:12">
+    <row r="221" spans="10:13">
       <c r="J221" t="str">
         <f t="shared" si="10"/>
         <v>BCBDD</v>
@@ -4284,7 +4699,7 @@
         <v>BCBDDB</v>
       </c>
     </row>
-    <row r="222" spans="10:12">
+    <row r="222" spans="10:13">
       <c r="J222" t="str">
         <f t="shared" si="10"/>
         <v>CCBDD</v>
@@ -4294,7 +4709,7 @@
         <v>CCBDDB</v>
       </c>
     </row>
-    <row r="223" spans="10:12">
+    <row r="223" spans="10:13">
       <c r="J223" t="str">
         <f t="shared" si="10"/>
         <v>DCBDD</v>
@@ -4304,7 +4719,7 @@
         <v>DCBDDB</v>
       </c>
     </row>
-    <row r="224" spans="10:12">
+    <row r="224" spans="10:13">
       <c r="J224" t="str">
         <f t="shared" si="10"/>
         <v>BDBDD</v>
@@ -4434,7 +4849,7 @@
         <v>BBDDDB</v>
       </c>
       <c r="M236" t="s">
-        <v>14</v>
+        <v>130</v>
       </c>
     </row>
     <row r="237" spans="10:13">
@@ -4513,7 +4928,7 @@
         <v>DDDDD</v>
       </c>
       <c r="K244" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="L244" t="str">
         <f t="shared" si="11"/>
@@ -4784,100 +5199,103 @@
         <v>CDCCBC</v>
       </c>
     </row>
-    <row r="289" spans="12:12">
+    <row r="289" spans="12:13">
       <c r="L289" t="str">
         <f t="shared" si="13"/>
         <v>DDCCBC</v>
       </c>
     </row>
-    <row r="290" spans="12:12">
+    <row r="290" spans="12:13">
       <c r="L290" t="str">
         <f t="shared" si="13"/>
         <v>BBDCBC</v>
       </c>
     </row>
-    <row r="291" spans="12:12">
+    <row r="291" spans="12:13">
       <c r="L291" t="str">
         <f t="shared" si="13"/>
         <v>CBDCBC</v>
       </c>
     </row>
-    <row r="292" spans="12:12">
+    <row r="292" spans="12:13">
       <c r="L292" t="str">
         <f t="shared" si="13"/>
         <v>DBDCBC</v>
       </c>
     </row>
-    <row r="293" spans="12:12">
+    <row r="293" spans="12:13">
       <c r="L293" t="str">
         <f t="shared" si="13"/>
         <v>BCDCBC</v>
       </c>
     </row>
-    <row r="294" spans="12:12">
+    <row r="294" spans="12:13">
       <c r="L294" t="str">
         <f t="shared" si="13"/>
         <v>CCDCBC</v>
       </c>
     </row>
-    <row r="295" spans="12:12">
+    <row r="295" spans="12:13">
       <c r="L295" t="str">
         <f t="shared" si="13"/>
         <v>DCDCBC</v>
       </c>
     </row>
-    <row r="296" spans="12:12">
+    <row r="296" spans="12:13">
       <c r="L296" t="str">
         <f t="shared" si="13"/>
         <v>BDDCBC</v>
       </c>
     </row>
-    <row r="297" spans="12:12">
+    <row r="297" spans="12:13">
       <c r="L297" t="str">
         <f t="shared" si="13"/>
         <v>CDDCBC</v>
       </c>
     </row>
-    <row r="298" spans="12:12">
+    <row r="298" spans="12:13">
       <c r="L298" t="str">
         <f t="shared" si="13"/>
         <v>DDDCBC</v>
       </c>
     </row>
-    <row r="299" spans="12:12">
+    <row r="299" spans="12:13">
       <c r="L299" t="str">
         <f t="shared" si="13"/>
         <v>BBBDBC</v>
       </c>
     </row>
-    <row r="300" spans="12:12">
+    <row r="300" spans="12:13">
       <c r="L300" t="str">
         <f t="shared" si="13"/>
         <v>CBBDBC</v>
       </c>
     </row>
-    <row r="301" spans="12:12">
+    <row r="301" spans="12:13">
       <c r="L301" t="str">
         <f t="shared" si="13"/>
         <v>DBBDBC</v>
       </c>
     </row>
-    <row r="302" spans="12:12">
+    <row r="302" spans="12:13">
       <c r="L302" t="str">
         <f t="shared" si="13"/>
         <v>BCBDBC</v>
       </c>
     </row>
-    <row r="303" spans="12:12">
+    <row r="303" spans="12:13">
       <c r="L303" t="str">
         <f t="shared" si="13"/>
         <v>CCBDBC</v>
       </c>
     </row>
-    <row r="304" spans="12:12">
+    <row r="304" spans="12:13">
       <c r="L304" t="str">
         <f t="shared" si="13"/>
         <v>DCBDBC</v>
+      </c>
+      <c r="M304" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="305" spans="12:13">
@@ -4921,12 +5339,18 @@
         <f t="shared" si="13"/>
         <v>BCCDBC</v>
       </c>
+      <c r="M311" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="312" spans="12:13">
       <c r="L312" t="str">
         <f t="shared" si="13"/>
         <v>CCCDBC</v>
       </c>
+      <c r="M312" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="313" spans="12:13">
       <c r="L313" t="str">
@@ -4958,7 +5382,7 @@
         <v>BBDDBC</v>
       </c>
       <c r="M317" t="s">
-        <v>33</v>
+        <v>147</v>
       </c>
     </row>
     <row r="318" spans="12:13">
@@ -5447,7 +5871,7 @@
         <v>BBDDCC</v>
       </c>
       <c r="M398" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="399" spans="12:13">
@@ -6422,7 +6846,7 @@
         <v>BBDDBD</v>
       </c>
       <c r="M560" t="s">
-        <v>27</v>
+        <v>141</v>
       </c>
     </row>
     <row r="561" spans="12:12">
@@ -6911,7 +7335,7 @@
         <v>BBDDCD</v>
       </c>
       <c r="M641" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
     </row>
     <row r="642" spans="12:13">
@@ -7448,10 +7872,11 @@
         <v>DDDDDD</v>
       </c>
       <c r="M730" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="M642:M1048576 N1:XFD1048576 M1:M316 M318:M640 A1:L1048576">
     <cfRule type="cellIs" dxfId="1" priority="0" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
Ideas of features: Adding intensity-sensitive color vision characteristics
</commit_message>
<xml_diff>
--- a/ideas/creatureFeatures.xlsx
+++ b/ideas/creatureFeatures.xlsx
@@ -20,7 +20,139 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="234">
+  <si>
+    <t>Enable vision for green in high intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision += [(0, 0), (-100, 100), (0, 0)] in high intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDCBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDDBC, DDDBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BDDCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBDDBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBBBBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stops high level of blue in high intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision blue capped (upper) at 3 in high intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Night lids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extend lower cap for all colors in low intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision += [(-1, 0), (-1, 0) (-1, 0)] in low intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stripped lids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mix up the visible colors during the day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implify low level colors during the night</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shift values for each color vision to the right (values for blue become for red, etc) in high intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision = [(tuple3), (tuple1), (tuple2)] in high intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marron lids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stops blue light in the night</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stops all blue in low intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorVision += [(0, 0), (0, 0), (-100, -100)] in low intensity light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ultragreen lids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boosts green vision in the day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Example long</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -234,6 +366,14 @@
   </si>
   <si>
     <t>VI8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day blue lids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shutters high levels of blue during the day</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1225,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1245,585 +1385,685 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>147</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="14" customHeight="1" thickTop="1">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>111</v>
+        <v>146</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="E5" t="s">
-        <v>197</v>
+        <v>232</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>198</v>
+        <v>233</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="D7" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="F7" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="E8" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>228</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="E9" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>200</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
       <c r="D10" t="s">
-        <v>184</v>
+        <v>219</v>
       </c>
       <c r="E10" t="s">
-        <v>185</v>
+        <v>220</v>
       </c>
       <c r="F10" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>186</v>
+        <v>221</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
       <c r="D11" t="s">
-        <v>188</v>
+        <v>223</v>
       </c>
       <c r="E11" t="s">
-        <v>183</v>
+        <v>218</v>
       </c>
       <c r="F11" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>202</v>
       </c>
       <c r="C12" t="s">
-        <v>190</v>
+        <v>225</v>
       </c>
       <c r="D12" t="s">
-        <v>191</v>
+        <v>226</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>227</v>
       </c>
       <c r="B13" t="s">
-        <v>168</v>
+        <v>203</v>
       </c>
       <c r="C13" t="s">
-        <v>194</v>
+        <v>229</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
+        <v>230</v>
       </c>
       <c r="E13" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>196</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>204</v>
       </c>
       <c r="C14" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
       <c r="D14" t="s">
-        <v>162</v>
+        <v>197</v>
       </c>
       <c r="E14" t="s">
-        <v>163</v>
+        <v>198</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>199</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
-        <v>172</v>
+        <v>207</v>
       </c>
       <c r="D15" t="s">
-        <v>173</v>
+        <v>208</v>
       </c>
       <c r="E15" t="s">
-        <v>174</v>
+        <v>209</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
       <c r="B16" t="s">
-        <v>175</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>176</v>
+        <v>211</v>
       </c>
       <c r="D16" t="s">
-        <v>177</v>
+        <v>212</v>
       </c>
       <c r="E16" t="s">
-        <v>178</v>
+        <v>213</v>
       </c>
       <c r="F16" t="s">
-        <v>161</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>180</v>
+        <v>215</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>216</v>
       </c>
       <c r="C17" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="E17" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>143</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>39</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" t="s">
-        <v>145</v>
-      </c>
-      <c r="D23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" t="s">
-        <v>60</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="C25" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" t="s">
         <v>63</v>
       </c>
-      <c r="D25" t="s">
-        <v>64</v>
-      </c>
       <c r="E25" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="F25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" t="s">
         <v>74</v>
-      </c>
-      <c r="C27" t="s">
-        <v>137</v>
-      </c>
-      <c r="D27" t="s">
-        <v>138</v>
-      </c>
-      <c r="E27" t="s">
-        <v>139</v>
-      </c>
-      <c r="F27" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>147</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="E28" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="F28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" t="s">
-        <v>122</v>
-      </c>
-      <c r="F29" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" t="s">
+        <v>140</v>
+      </c>
+      <c r="F30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" t="s">
+        <v>172</v>
+      </c>
+      <c r="D32" t="s">
+        <v>173</v>
+      </c>
+      <c r="E32" t="s">
+        <v>174</v>
+      </c>
+      <c r="F32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" t="s">
+        <v>183</v>
+      </c>
+      <c r="D33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" t="s">
+        <v>161</v>
+      </c>
+      <c r="D35" t="s">
+        <v>162</v>
+      </c>
+      <c r="E35" t="s">
+        <v>163</v>
+      </c>
+      <c r="F35" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" t="s">
         <v>127</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" t="s">
+        <v>169</v>
+      </c>
+      <c r="D44" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" t="s">
         <v>128</v>
       </c>
-      <c r="F30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
+      <c r="F44" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" t="s">
         <v>135</v>
       </c>
-      <c r="B38" t="s">
-        <v>132</v>
-      </c>
-      <c r="C38" t="s">
-        <v>131</v>
-      </c>
-      <c r="D38" t="s">
-        <v>118</v>
-      </c>
-      <c r="E38" t="s">
-        <v>92</v>
-      </c>
-      <c r="F38" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
+      <c r="D45" t="s">
         <v>136</v>
       </c>
-      <c r="B39" t="s">
-        <v>133</v>
-      </c>
-      <c r="C39" t="s">
-        <v>134</v>
-      </c>
-      <c r="D39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E39" t="s">
-        <v>93</v>
-      </c>
-      <c r="F39" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>98</v>
-      </c>
-      <c r="B40" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" t="s">
-        <v>100</v>
-      </c>
-      <c r="D40" t="s">
-        <v>101</v>
-      </c>
-      <c r="E40" t="s">
-        <v>102</v>
-      </c>
-      <c r="F40" t="s">
-        <v>103</v>
+      <c r="E45" t="s">
+        <v>137</v>
+      </c>
+      <c r="F45" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1843,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:P730"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="M306" sqref="M306"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="K257" sqref="K257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1860,7 +2100,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1881,42 +2121,42 @@
         <v>6</v>
       </c>
       <c r="N1" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="O1" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="P1" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="B2" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)))</f>
         <v>BB</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="F2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)) )</f>
         <v>BBB</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)), IF(MOD(QUOTIENT(ROW() - 2,27),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)) )</f>
         <v>BBBB</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J2" t="str">
         <f>CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,27),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,81),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,81), 3) = 1, $B$3, $B$4)) )</f>
@@ -1936,22 +2176,22 @@
       </c>
       <c r="P2">
         <f>COUNTIF($C$2:$C$4,"*")+O2+COUNTIF($E$2:$E$10,"*")+COUNTIF($G$2:$G$28,"*")+COUNTIF($I$2:$I$82,"*")+COUNTIF($K$2:$K$244,"*")+COUNTIF($M$2:$M$730,"*") - N2 - O2</f>
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="B3" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D9" si="0">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)))</f>
         <v>CB</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F27" si="1">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)) )</f>
@@ -1972,17 +2212,17 @@
     </row>
     <row r="4" spans="1:16">
       <c r="B4" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>DB</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -2007,7 +2247,7 @@
         <v>BC</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -2018,14 +2258,14 @@
         <v>BCBB</v>
       </c>
       <c r="I5" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="3"/>
         <v>BCBBB</v>
       </c>
       <c r="K5" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="4"/>
@@ -2038,7 +2278,7 @@
         <v>CC</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
@@ -2063,7 +2303,7 @@
         <v>DC</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
@@ -2088,7 +2328,7 @@
         <v>BD</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
@@ -2113,7 +2353,7 @@
         <v>CD</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -2138,7 +2378,7 @@
         <v>DD</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -2163,7 +2403,7 @@
         <v>BBC</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="2"/>
@@ -2224,14 +2464,14 @@
         <v>BCCB</v>
       </c>
       <c r="I14" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="3"/>
         <v>BCCBB</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="4"/>
@@ -2334,7 +2574,7 @@
         <v>BBD</v>
       </c>
       <c r="G20" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="2"/>
@@ -2395,14 +2635,14 @@
         <v>BCDB</v>
       </c>
       <c r="I23" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="3"/>
         <v>BCDBB</v>
       </c>
       <c r="K23" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="4"/>
@@ -2487,7 +2727,7 @@
         <v>DDD</v>
       </c>
       <c r="G28" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="2"/>
@@ -2508,7 +2748,7 @@
         <v>BBBC</v>
       </c>
       <c r="I29" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="3"/>
@@ -2561,7 +2801,7 @@
         <v>BCBCBB</v>
       </c>
       <c r="M32" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="8:12">
@@ -2640,7 +2880,7 @@
         <v>BBCC</v>
       </c>
       <c r="I38" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="3"/>
@@ -2815,7 +3055,7 @@
         <v>BCDCB</v>
       </c>
       <c r="K50" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="L50" t="str">
         <f t="shared" si="4"/>
@@ -2859,6 +3099,9 @@
         <f t="shared" si="3"/>
         <v>BDDCB</v>
       </c>
+      <c r="K53" t="s">
+        <v>7</v>
+      </c>
       <c r="L53" t="str">
         <f t="shared" si="4"/>
         <v>BDDCBB</v>
@@ -2898,7 +3141,7 @@
         <v>BBBD</v>
       </c>
       <c r="I56" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="J56" t="str">
         <f t="shared" si="3"/>
@@ -2951,7 +3194,7 @@
         <v>BCBDBB</v>
       </c>
       <c r="M59" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="8:13">
@@ -3030,7 +3273,7 @@
         <v>BBCD</v>
       </c>
       <c r="I65" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="J65" t="str">
         <f t="shared" si="3"/>
@@ -3083,7 +3326,7 @@
         <v>BCCDBB</v>
       </c>
       <c r="M68" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="8:13">
@@ -3100,7 +3343,7 @@
         <v>CCCDBB</v>
       </c>
       <c r="M69" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="8:13">
@@ -3117,7 +3360,7 @@
         <v>DCCDBB</v>
       </c>
       <c r="M70" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" spans="8:13">
@@ -3148,7 +3391,7 @@
         <v>CDCDBB</v>
       </c>
       <c r="M72" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="8:13">
@@ -3171,7 +3414,7 @@
         <v>BBDD</v>
       </c>
       <c r="I74" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="J74" t="str">
         <f t="shared" si="6"/>
@@ -3224,7 +3467,7 @@
         <v>BCDDBB</v>
       </c>
       <c r="M77" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="8:13">
@@ -3289,7 +3532,7 @@
         <v>DDDD</v>
       </c>
       <c r="I82" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="J82" t="str">
         <f t="shared" si="6"/>
@@ -3465,6 +3708,9 @@
         <f t="shared" si="6"/>
         <v>CDCBC</v>
       </c>
+      <c r="K99" t="s">
+        <v>2</v>
+      </c>
       <c r="L99" t="str">
         <f t="shared" si="7"/>
         <v>CDCBCB</v>
@@ -3555,6 +3801,9 @@
         <f t="shared" si="6"/>
         <v>CDDBC</v>
       </c>
+      <c r="K108" t="s">
+        <v>4</v>
+      </c>
       <c r="L108" t="str">
         <f t="shared" si="7"/>
         <v>CDDBCB</v>
@@ -3565,6 +3814,9 @@
         <f t="shared" si="6"/>
         <v>DDDBC</v>
       </c>
+      <c r="K109" t="s">
+        <v>4</v>
+      </c>
       <c r="L109" t="str">
         <f t="shared" si="7"/>
         <v>DDDBCB</v>
@@ -4410,7 +4662,7 @@
         <v>DBBCDB</v>
       </c>
       <c r="M193" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="194" spans="10:13">
@@ -4533,7 +4785,7 @@
         <v>DCCCDB</v>
       </c>
       <c r="M205" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="206" spans="10:13">
@@ -4656,7 +4908,7 @@
         <v>DDDCDB</v>
       </c>
       <c r="M217" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="218" spans="10:13">
@@ -4849,7 +5101,7 @@
         <v>BBDDDB</v>
       </c>
       <c r="M236" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
     </row>
     <row r="237" spans="10:13">
@@ -4892,7 +5144,7 @@
         <v>CCDDDB</v>
       </c>
     </row>
-    <row r="241" spans="10:12">
+    <row r="241" spans="10:13">
       <c r="J241" t="str">
         <f t="shared" si="10"/>
         <v>DCDDD</v>
@@ -4902,7 +5154,7 @@
         <v>DCDDDB</v>
       </c>
     </row>
-    <row r="242" spans="10:12">
+    <row r="242" spans="10:13">
       <c r="J242" t="str">
         <f t="shared" si="10"/>
         <v>BDDDD</v>
@@ -4912,7 +5164,7 @@
         <v>BDDDDB</v>
       </c>
     </row>
-    <row r="243" spans="10:12">
+    <row r="243" spans="10:13">
       <c r="J243" t="str">
         <f t="shared" si="10"/>
         <v>CDDDD</v>
@@ -4922,86 +5174,89 @@
         <v>CDDDDB</v>
       </c>
     </row>
-    <row r="244" spans="10:12">
+    <row r="244" spans="10:13">
       <c r="J244" t="str">
         <f t="shared" si="10"/>
         <v>DDDDD</v>
       </c>
       <c r="K244" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="L244" t="str">
         <f t="shared" si="11"/>
         <v>DDDDDB</v>
       </c>
     </row>
-    <row r="245" spans="10:12">
+    <row r="245" spans="10:13">
       <c r="L245" t="str">
         <f t="shared" ref="L245:L258" si="12">CONCATENATE(IF(MOD(ROW() - 2,3) = 0, $B$2, IF(MOD(ROW() - 2, 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,3),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,3), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,9),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,9), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,27), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,81),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,81), 3) = 1, $B$3, $B$4)),IF(MOD(QUOTIENT(ROW() - 2,243),3) = 0, $B$2, IF(MOD(QUOTIENT(ROW() - 2,243), 3) = 1, $B$3, $B$4)))</f>
         <v>BBBBBC</v>
       </c>
     </row>
-    <row r="246" spans="10:12">
+    <row r="246" spans="10:13">
       <c r="L246" t="str">
         <f t="shared" si="12"/>
         <v>CBBBBC</v>
       </c>
-    </row>
-    <row r="247" spans="10:12">
+      <c r="M246" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="247" spans="10:13">
       <c r="L247" t="str">
         <f t="shared" si="12"/>
         <v>DBBBBC</v>
       </c>
     </row>
-    <row r="248" spans="10:12">
+    <row r="248" spans="10:13">
       <c r="L248" t="str">
         <f t="shared" si="12"/>
         <v>BCBBBC</v>
       </c>
     </row>
-    <row r="249" spans="10:12">
+    <row r="249" spans="10:13">
       <c r="L249" t="str">
         <f t="shared" si="12"/>
         <v>CCBBBC</v>
       </c>
     </row>
-    <row r="250" spans="10:12">
+    <row r="250" spans="10:13">
       <c r="L250" t="str">
         <f t="shared" si="12"/>
         <v>DCBBBC</v>
       </c>
     </row>
-    <row r="251" spans="10:12">
+    <row r="251" spans="10:13">
       <c r="L251" t="str">
         <f t="shared" si="12"/>
         <v>BDBBBC</v>
       </c>
     </row>
-    <row r="252" spans="10:12">
+    <row r="252" spans="10:13">
       <c r="L252" t="str">
         <f t="shared" si="12"/>
         <v>CDBBBC</v>
       </c>
     </row>
-    <row r="253" spans="10:12">
+    <row r="253" spans="10:13">
       <c r="L253" t="str">
         <f t="shared" si="12"/>
         <v>DDBBBC</v>
       </c>
     </row>
-    <row r="254" spans="10:12">
+    <row r="254" spans="10:13">
       <c r="L254" t="str">
         <f t="shared" si="12"/>
         <v>BBCBBC</v>
       </c>
     </row>
-    <row r="255" spans="10:12">
+    <row r="255" spans="10:13">
       <c r="L255" t="str">
         <f t="shared" si="12"/>
         <v>CBCBBC</v>
       </c>
     </row>
-    <row r="256" spans="10:12">
+    <row r="256" spans="10:13">
       <c r="L256" t="str">
         <f t="shared" si="12"/>
         <v>DBCBBC</v>
@@ -5295,7 +5550,7 @@
         <v>DCBDBC</v>
       </c>
       <c r="M304" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
     </row>
     <row r="305" spans="12:13">
@@ -5340,7 +5595,7 @@
         <v>BCCDBC</v>
       </c>
       <c r="M311" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
     </row>
     <row r="312" spans="12:13">
@@ -5349,7 +5604,7 @@
         <v>CCCDBC</v>
       </c>
       <c r="M312" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="313" spans="12:13">
@@ -5382,7 +5637,7 @@
         <v>BBDDBC</v>
       </c>
       <c r="M317" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
     </row>
     <row r="318" spans="12:13">
@@ -5390,6 +5645,9 @@
         <f t="shared" si="13"/>
         <v>CBDDBC</v>
       </c>
+      <c r="M318" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="319" spans="12:13">
       <c r="L319" t="str">
@@ -5871,7 +6129,7 @@
         <v>BBDDCC</v>
       </c>
       <c r="M398" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
     </row>
     <row r="399" spans="12:13">
@@ -6846,7 +7104,7 @@
         <v>BBDDBD</v>
       </c>
       <c r="M560" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
     </row>
     <row r="561" spans="12:12">
@@ -7335,7 +7593,7 @@
         <v>BBDDCD</v>
       </c>
       <c r="M641" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="642" spans="12:13">
@@ -7872,13 +8130,13 @@
         <v>DDDDDD</v>
       </c>
       <c r="M730" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="M642:M1048576 N1:XFD1048576 M1:M316 M318:M640 A1:L1048576">
+  <conditionalFormatting sqref="M642:M1048576 N1:XFD1048576 A1:L1048576 M318:M640 M1:M316">
     <cfRule type="cellIs" dxfId="1" priority="0" stopIfTrue="1" operator="equal">
       <formula>"VOID"</formula>
     </cfRule>

</xml_diff>